<commit_message>
added image and sheetdata to html
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\phosphorus\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adm\Desktop\dir\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898A4E6D-2CB8-4518-B404-2AE8FDF557D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>https://google.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>B</t>
   </si>
@@ -38,11 +34,17 @@
   <si>
     <t>M</t>
   </si>
+  <si>
+    <t>https://github.com/NaturalIntelligence/fast-xml-parser/blob/HEAD/docs/v4/2.XMLparseOptions.md</t>
+  </si>
+  <si>
+    <t>https://google.com/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -81,9 +83,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -107,15 +115,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>809625</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>428625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1722120</xdr:colOff>
+      <xdr:colOff>2531745</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1076325</xdr:rowOff>
+      <xdr:rowOff>1504950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -144,7 +152,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="809625" y="428625"/>
           <a:ext cx="1722120" cy="1076325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -159,13 +167,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>981076</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2257426</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1635692</xdr:rowOff>
+      <xdr:rowOff>1692842</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -194,7 +202,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="981076" y="1409701"/>
+          <a:off x="981076" y="2105026"/>
           <a:ext cx="1276350" cy="1569016"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -207,15 +215,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
+      <xdr:colOff>628650</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>466725</xdr:rowOff>
+      <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2975185</xdr:colOff>
+      <xdr:colOff>2541165</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>2476500</xdr:rowOff>
+      <xdr:rowOff>1571625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -244,8 +252,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="133350" y="3486150"/>
-          <a:ext cx="2841835" cy="2009775"/>
+          <a:off x="628650" y="4038600"/>
+          <a:ext cx="1912515" cy="1352550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -519,48 +527,424 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" ht="156" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1">
+    </row>
+    <row r="2" spans="2:5" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
+      <c r="C2" s="3">
+        <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="2:4" ht="132" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="2:5" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" ht="240.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="2:5" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="2:5" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="2"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="2"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="2"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="2"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="2"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="2"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="2"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="2"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="2"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="2"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="2"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="2"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" s="2"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="2"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="2"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="2"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{AA36F59D-403F-495B-A10A-1FC82B24098A}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{0F38B628-4BE2-4417-A577-1AF35358200D}"/>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
processing of empty cells
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>B</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>https://google.com/</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -530,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,19 +575,27 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="3">
+        <v>45646</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="2:5" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="2:5" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
@@ -605,12 +619,16 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3">
+        <v>5</v>
+      </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3">
+        <v>546</v>
+      </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>